<commit_message>
Adding example datasets and metadata
</commit_message>
<xml_diff>
--- a/Datasets/Ebert_Dataset.xlsx
+++ b/Datasets/Ebert_Dataset.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0e630846ca949a3/Documents/CompBio_Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{E74ED9F8-BEDF-4DCF-A57E-E7511F27356E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48AD0E5C-1975-478A-BDE7-FB2D82E978C0}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{E74ED9F8-BEDF-4DCF-A57E-E7511F27356E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A23B66F-25AA-4E19-8274-FBF56D25C05C}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t># TITLE: Brief title for entire data set</t>
   </si>
@@ -130,45 +141,6 @@
   </si>
   <si>
     <t>Latest Update</t>
-  </si>
-  <si>
-    <t>ID_REF</t>
-  </si>
-  <si>
-    <t>GSM2299032</t>
-  </si>
-  <si>
-    <t>GSM2299033</t>
-  </si>
-  <si>
-    <t>GSM2299034</t>
-  </si>
-  <si>
-    <t>GSM2299035</t>
-  </si>
-  <si>
-    <t>GSM2299036</t>
-  </si>
-  <si>
-    <t>GSM2299037</t>
-  </si>
-  <si>
-    <t>GSM2299038</t>
-  </si>
-  <si>
-    <t>GSM2299039</t>
-  </si>
-  <si>
-    <t>GSM2299040</t>
-  </si>
-  <si>
-    <t>GSM2299041</t>
-  </si>
-  <si>
-    <t>GSM2299042</t>
-  </si>
-  <si>
-    <t>GSM2299043</t>
   </si>
   <si>
     <t>GSMXXXXXXX: Code for particular sample group</t>
@@ -530,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -674,13 +646,13 @@
         <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
@@ -749,64 +721,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>35</v>
-      </c>
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D35" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" t="s">
-        <v>39</v>
-      </c>
-      <c r="F35" t="s">
-        <v>40</v>
-      </c>
-      <c r="G35" t="s">
-        <v>41</v>
-      </c>
-      <c r="H35" t="s">
-        <v>42</v>
-      </c>
-      <c r="I35" t="s">
-        <v>43</v>
-      </c>
-      <c r="J35" t="s">
-        <v>44</v>
-      </c>
-      <c r="K35" t="s">
-        <v>45</v>
-      </c>
-      <c r="L35" t="s">
-        <v>46</v>
-      </c>
-      <c r="M35" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add example dataset page and links on index page
</commit_message>
<xml_diff>
--- a/Datasets/Ebert_Dataset.xlsx
+++ b/Datasets/Ebert_Dataset.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0e630846ca949a3/Documents/CompBio_Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d0e630846ca949a3/Documents/R/Bio381/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="50" documentId="8_{E74ED9F8-BEDF-4DCF-A57E-E7511F27356E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A23B66F-25AA-4E19-8274-FBF56D25C05C}"/>
@@ -504,8 +504,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>